<commit_message>
Software: Notaus und Startbutton funktionieren, Dokumentation stand 04.12.2023
</commit_message>
<xml_diff>
--- a/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_2.xlsx
+++ b/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vds66\redirectedfolders$\students\190049\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ESY_Car\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58D1C6E-7AA8-4B2F-BD6E-4B25C7A67F63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAB0683-6CAF-4295-A8D6-42596691DB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="643" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="643" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="234">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1123,13 +1123,22 @@
     <t>gefehlt</t>
   </si>
   <si>
-    <t>Drähte neu verdrahtet</t>
-  </si>
-  <si>
-    <t>Fehler gesucht und behoben einen Kurzschluss und einen Kabelbruch behoben</t>
-  </si>
-  <si>
-    <t>Softwareoptimierung button einlesen so dass wenn man in drückt der Motor läuft und wenn der Button nicht gedrückt wird nicht</t>
+    <t>Drähte neu verlegt</t>
+  </si>
+  <si>
+    <t>Fehler gesucht und behoben, einen Kurzschluss und einen Kabelbruch beim Motor behoben</t>
+  </si>
+  <si>
+    <t>Softwareoptimierung Startbutton funktioniert, Notaus nicht</t>
+  </si>
+  <si>
+    <t>Softwareoptimierung Startbutton funktioniert und Notaus auch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versucht die Sensoren in den Code zu integrieren (nicht erfolgreich) </t>
+  </si>
+  <si>
+    <t>Drähte an die Sensoren gelötet und die Sensoren an das Auto gebaut</t>
   </si>
 </sst>
 </file>
@@ -1849,12 +1858,51 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1864,36 +1912,6 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1917,15 +1935,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2412,14 +2421,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="124" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2468,10 +2477,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="111" t="s">
+      <c r="E7" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="119"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2482,8 +2491,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2494,8 +2503,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2506,8 +2515,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2518,8 +2527,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2540,49 +2549,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="117"/>
+      <c r="B16" s="123"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
-      <c r="E18" s="117"/>
-      <c r="F18" s="117"/>
+      <c r="B18" s="123"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="123"/>
+      <c r="F18" s="123"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2595,64 +2604,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="111" t="s">
+      <c r="A26" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111" t="s">
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
+      <c r="E26" s="119"/>
+      <c r="F26" s="119"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="119" t="s">
+      <c r="A27" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="124"/>
+      <c r="B27" s="114"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="118" t="s">
+      <c r="A28" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="119" t="s">
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="114" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="114"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="120"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2663,16 +2682,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2685,7 +2694,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,11 +2703,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="129" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
@@ -2794,20 +2803,26 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="134">
+      <c r="A11" s="111">
         <v>45257</v>
       </c>
-      <c r="B11" s="135">
+      <c r="B11" s="112">
         <v>3</v>
       </c>
-      <c r="C11" s="133" t="s">
+      <c r="C11" s="110" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="105"/>
+      <c r="A12" s="111">
+        <v>45264</v>
+      </c>
+      <c r="B12" s="112">
+        <v>3</v>
+      </c>
+      <c r="C12" s="110" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
@@ -2989,29 +3004,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="125"/>
+      <c r="C3" s="128"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="125"/>
+      <c r="C4" s="128"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="125"/>
+      <c r="C5" s="128"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3224,7 +3239,7 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3236,11 +3251,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3248,18 +3263,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -3529,14 +3544,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3814,8 +3829,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3829,16 +3844,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4012,10 +4027,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="56">
+        <v>2</v>
+      </c>
+      <c r="F11" s="56">
         <v>1</v>
-      </c>
-      <c r="F11" s="56">
-        <v>0</v>
       </c>
       <c r="G11" s="58">
         <v>45278</v>
@@ -4035,10 +4050,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" s="56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G12" s="58">
         <v>45278</v>
@@ -4083,15 +4098,17 @@
         <v>1</v>
       </c>
       <c r="E14" s="56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="56">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G14" s="58">
         <v>45250</v>
       </c>
-      <c r="H14" s="56"/>
+      <c r="H14" s="58">
+        <v>45264</v>
+      </c>
       <c r="I14" s="59"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4401,11 +4418,11 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="I35" s="71"/>
     </row>
@@ -4451,19 +4468,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="132" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -5127,16 +5144,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="129" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -5912,71 +5929,71 @@
       <c r="A21" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="131" t="s">
+      <c r="B21" s="134" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="131"/>
-      <c r="D21" s="131"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="132" t="s">
+      <c r="B22" s="135" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132"/>
+      <c r="C22" s="135"/>
+      <c r="D22" s="135"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="132" t="s">
+      <c r="B23" s="135" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
+      <c r="C23" s="135"/>
+      <c r="D23" s="135"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="132" t="s">
+      <c r="B24" s="135" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="135"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="130"/>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
+      <c r="B25" s="133"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="130"/>
-      <c r="C26" s="130"/>
-      <c r="D26" s="130"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="130"/>
-      <c r="D27" s="130"/>
+      <c r="B27" s="133"/>
+      <c r="C27" s="133"/>
+      <c r="D27" s="133"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130"/>
-      <c r="D28" s="130"/>
+      <c r="B28" s="133"/>
+      <c r="C28" s="133"/>
+      <c r="D28" s="133"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="130"/>
-      <c r="C29" s="130"/>
-      <c r="D29" s="130"/>
+      <c r="B29" s="133"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6013,8 +6030,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6026,11 +6043,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="129" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -6147,13 +6164,13 @@
         <v>45257</v>
       </c>
       <c r="B13" s="41">
-        <v>0.66700000000000004</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>45257</v>
       </c>
@@ -6165,19 +6182,37 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="2"/>
+      <c r="A15" s="40">
+        <v>45264</v>
+      </c>
+      <c r="B15" s="41">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="40">
+        <v>45264</v>
+      </c>
+      <c r="B16" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>45264</v>
+      </c>
+      <c r="B17" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>

</xml_diff>

<commit_message>
Clean-up whole structure - let git create your file versions :-)
</commit_message>
<xml_diff>
--- a/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_2.xlsx
+++ b/Dokumentation/Projekt-Steuerung_Autonom-Fahrendes-Auto_Gruppe_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ESY_Car\Dokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\5 AHEL\Autonomes_Auto\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAB0683-6CAF-4295-A8D6-42596691DB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0DB53F-B46A-4869-A720-F88EAE84BDEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="643" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="643" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="245">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1139,6 +1139,39 @@
   </si>
   <si>
     <t>Drähte an die Sensoren gelötet und die Sensoren an das Auto gebaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabelbruch beim an- uns ausschalter </t>
+  </si>
+  <si>
+    <t>Versucht die Sensoren in den Code zu integrieren (nicht erfolgreich), Probleme mit den Sensoren werden nicht im Code erkannt</t>
+  </si>
+  <si>
+    <t>Dritten Sharp sensor an Pin A2 angeschloßen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourcetree eingerichtet </t>
+  </si>
+  <si>
+    <t>Versucht in den Code eine Mittelregelung zu integrieren mittels Sharp Sensoren nicht erfolgreich</t>
+  </si>
+  <si>
+    <t>Stabile Sensordaten erfassen</t>
+  </si>
+  <si>
+    <t>Probleme mit der Erkennung vom Arduinoboard beim Pc</t>
+  </si>
+  <si>
+    <t>Probleme mit der Erkennung vom Arduinoboard beim Pc, erfolgreich</t>
+  </si>
+  <si>
+    <t>Einen Code entwickelt der die Sensordaten stabil erfasst, erfolgreich</t>
+  </si>
+  <si>
+    <t>Stabile Sensordatenerfassung auf den Seiten(erfolgreich), Stabile Sensordatenerfassung Mitte(nicht erfolgreich)</t>
+  </si>
+  <si>
+    <t>Sensordatenerfassung Mitte und Seite(erfolgreich), mittels Sensordaten die Motoren ansteuern(nicht erfolgreich)</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1570,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1866,6 +1899,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2421,14 +2457,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2477,10 +2513,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="119"/>
+      <c r="F7" s="120"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2491,8 +2527,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2503,8 +2539,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2515,8 +2551,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="127"/>
-      <c r="F10" s="127"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2527,8 +2563,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="121"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2549,49 +2585,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="122"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="122"/>
-      <c r="F15" s="122"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="123"/>
-      <c r="C16" s="123"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="123"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="124"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="123"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
-      <c r="E19" s="117"/>
-      <c r="F19" s="117"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2604,61 +2640,61 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="118" t="s">
+      <c r="A23" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="119" t="s">
+      <c r="A26" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="119"/>
-      <c r="C26" s="119"/>
-      <c r="D26" s="119" t="s">
+      <c r="B26" s="120"/>
+      <c r="C26" s="120"/>
+      <c r="D26" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="119"/>
-      <c r="F26" s="119"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="120"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="114" t="s">
+      <c r="A27" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="121"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="113" t="s">
+      <c r="A28" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="113"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="114" t="s">
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="E28" s="114"/>
-      <c r="F28" s="114"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="115" t="s">
+      <c r="A29" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="115"/>
-      <c r="C29" s="115"/>
-      <c r="D29" s="116"/>
-      <c r="E29" s="116"/>
-      <c r="F29" s="116"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -2693,8 +2729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,11 +2739,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
@@ -2825,44 +2861,92 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="105"/>
+      <c r="A13" s="111">
+        <v>45271</v>
+      </c>
+      <c r="B13" s="112">
+        <v>3</v>
+      </c>
+      <c r="C13" s="110" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="105"/>
+      <c r="A14" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B14" s="41">
+        <v>0.16</v>
+      </c>
+      <c r="C14" s="105" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="105"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="105"/>
+      <c r="A15" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B15" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="105" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B16" s="41">
+        <v>2.34</v>
+      </c>
+      <c r="C16" s="105" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="105"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="105"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="105"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="105"/>
+      <c r="A17" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B17" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="C17" s="105" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B18" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="105" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
+        <v>45306</v>
+      </c>
+      <c r="B19" s="41">
+        <v>3</v>
+      </c>
+      <c r="C19" s="105" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
+        <v>45313</v>
+      </c>
+      <c r="B20" s="41">
+        <v>3</v>
+      </c>
+      <c r="C20" s="105" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
@@ -2990,8 +3074,8 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3004,29 +3088,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="128"/>
+      <c r="C3" s="129"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="128"/>
+      <c r="C4" s="129"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="128"/>
+      <c r="C5" s="129"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3237,10 +3321,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,11 +3335,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3263,18 +3347,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="131" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="131"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="132"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -3321,7 +3405,9 @@
       <c r="B9" s="39">
         <v>45257</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="39">
+        <v>45278</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -3342,8 +3428,8 @@
       <c r="C11" s="41"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
+      <c r="A12" s="113" t="s">
+        <v>239</v>
       </c>
       <c r="B12" s="39">
         <v>45306</v>
@@ -3352,52 +3438,56 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="39">
-        <v>45320</v>
+        <v>45306</v>
       </c>
       <c r="C13" s="41"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="39">
+        <v>45320</v>
+      </c>
+      <c r="C14" s="41"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="39">
+      <c r="B15" s="39">
         <v>45341</v>
       </c>
-      <c r="C14" s="41"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B16" s="39">
         <v>45355</v>
       </c>
-      <c r="C15" s="41"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="41"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="39">
+      <c r="B17" s="39">
         <v>45362</v>
       </c>
-      <c r="C16" s="41"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="41"/>
       <c r="C17" s="41"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="41"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3407,12 +3497,12 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="41"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3422,12 +3512,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="40"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="41"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3506,9 +3596,14 @@
       <c r="C40" s="41"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3544,14 +3639,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3829,8 +3924,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,16 +3939,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4030,12 +4125,14 @@
         <v>2</v>
       </c>
       <c r="F11" s="56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="58">
         <v>45278</v>
       </c>
-      <c r="H11" s="58"/>
+      <c r="H11" s="58">
+        <v>45271</v>
+      </c>
       <c r="I11" s="59"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4053,12 +4150,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="58">
         <v>45278</v>
       </c>
-      <c r="H12" s="58"/>
+      <c r="H12" s="58">
+        <v>45271</v>
+      </c>
       <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
@@ -4148,10 +4247,18 @@
       <c r="D17" s="57">
         <v>5</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
+      <c r="E17" s="56">
+        <v>2</v>
+      </c>
+      <c r="F17" s="56">
+        <v>0</v>
+      </c>
+      <c r="G17" s="58">
+        <v>45278</v>
+      </c>
+      <c r="H17" s="58">
+        <v>45278</v>
+      </c>
       <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
@@ -4165,9 +4272,15 @@
       <c r="D18" s="57">
         <v>8</v>
       </c>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="58"/>
+      <c r="E18" s="56">
+        <v>4</v>
+      </c>
+      <c r="F18" s="56">
+        <v>2</v>
+      </c>
+      <c r="G18" s="58">
+        <v>45299</v>
+      </c>
       <c r="H18" s="56"/>
       <c r="I18" s="59"/>
     </row>
@@ -4182,9 +4295,15 @@
       <c r="D19" s="57">
         <v>3</v>
       </c>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="58"/>
+      <c r="E19" s="56">
+        <v>0</v>
+      </c>
+      <c r="F19" s="56">
+        <v>3</v>
+      </c>
+      <c r="G19" s="58">
+        <v>45313</v>
+      </c>
       <c r="H19" s="56"/>
       <c r="I19" s="59"/>
     </row>
@@ -4199,8 +4318,12 @@
       <c r="D20" s="62">
         <v>4</v>
       </c>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
+      <c r="E20" s="56">
+        <v>0</v>
+      </c>
+      <c r="F20" s="56">
+        <v>4</v>
+      </c>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
       <c r="I20" s="59"/>
@@ -4242,9 +4365,15 @@
       <c r="D23" s="64">
         <v>1</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="58"/>
+      <c r="E23" s="65">
+        <v>0</v>
+      </c>
+      <c r="F23" s="65">
+        <v>1</v>
+      </c>
+      <c r="G23" s="58">
+        <v>45278</v>
+      </c>
       <c r="H23" s="65"/>
       <c r="I23" s="66"/>
     </row>
@@ -4259,9 +4388,15 @@
       <c r="D24" s="108">
         <v>10</v>
       </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="58"/>
+      <c r="E24" s="65">
+        <v>0</v>
+      </c>
+      <c r="F24" s="65">
+        <v>10</v>
+      </c>
+      <c r="G24" s="58">
+        <v>44976</v>
+      </c>
       <c r="H24" s="65"/>
       <c r="I24" s="66"/>
     </row>
@@ -4276,9 +4411,15 @@
       <c r="D25" s="64">
         <v>3</v>
       </c>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="58"/>
+      <c r="E25" s="65">
+        <v>0</v>
+      </c>
+      <c r="F25" s="65">
+        <v>3</v>
+      </c>
+      <c r="G25" s="58">
+        <v>45341</v>
+      </c>
       <c r="H25" s="65"/>
       <c r="I25" s="66"/>
     </row>
@@ -4293,9 +4434,15 @@
       <c r="D26" s="64">
         <v>6</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="58"/>
+      <c r="E26" s="65">
+        <v>1</v>
+      </c>
+      <c r="F26" s="65">
+        <v>0</v>
+      </c>
+      <c r="G26" s="58">
+        <v>45348</v>
+      </c>
       <c r="H26" s="65"/>
       <c r="I26" s="66"/>
     </row>
@@ -4308,10 +4455,14 @@
       </c>
       <c r="C27" s="56"/>
       <c r="D27" s="108">
-        <v>6</v>
-      </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="65">
+        <v>0</v>
+      </c>
+      <c r="F27" s="65">
+        <v>0</v>
+      </c>
       <c r="G27" s="58"/>
       <c r="H27" s="65"/>
       <c r="I27" s="66"/>
@@ -4327,9 +4478,15 @@
       <c r="D28" s="108">
         <v>6</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="58"/>
+      <c r="E28" s="65">
+        <v>4</v>
+      </c>
+      <c r="F28" s="65">
+        <v>10</v>
+      </c>
+      <c r="G28" s="58">
+        <v>45355</v>
+      </c>
       <c r="H28" s="65"/>
       <c r="I28" s="66"/>
     </row>
@@ -4344,9 +4501,15 @@
       <c r="D29" s="57">
         <v>3</v>
       </c>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="58"/>
+      <c r="E29" s="56">
+        <v>0</v>
+      </c>
+      <c r="F29" s="56">
+        <v>0</v>
+      </c>
+      <c r="G29" s="58">
+        <v>45362</v>
+      </c>
       <c r="H29" s="56"/>
       <c r="I29" s="59"/>
     </row>
@@ -4361,9 +4524,15 @@
       <c r="D30" s="57">
         <v>2</v>
       </c>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="58"/>
+      <c r="E30" s="56">
+        <v>0</v>
+      </c>
+      <c r="F30" s="56">
+        <v>0</v>
+      </c>
+      <c r="G30" s="58">
+        <v>45367</v>
+      </c>
       <c r="H30" s="56"/>
       <c r="I30" s="59"/>
     </row>
@@ -4414,15 +4583,15 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="49">
         <f>SUM(D10:D34)</f>
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="I35" s="71"/>
     </row>
@@ -4468,19 +4637,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="133" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -5144,16 +5313,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -5685,7 +5854,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,13 +5931,13 @@
         <v>172</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C7" s="99" t="s">
         <v>170</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K7" s="96" t="s">
         <v>175</v>
@@ -5929,71 +6098,71 @@
       <c r="A21" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="B21" s="134" t="s">
+      <c r="B21" s="135" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
+      <c r="C21" s="135"/>
+      <c r="D21" s="135"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="B22" s="135" t="s">
+      <c r="B22" s="136" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="135"/>
-      <c r="D22" s="135"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="136"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="136" t="s">
         <v>191</v>
       </c>
-      <c r="C23" s="135"/>
-      <c r="D23" s="135"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="136"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="135" t="s">
+      <c r="B24" s="136" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="135"/>
-      <c r="D24" s="135"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="136"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="133"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="133"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="133"/>
-      <c r="C27" s="133"/>
-      <c r="D27" s="133"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="133"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="133"/>
+      <c r="B28" s="134"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="133"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="133"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6031,7 +6200,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C17:C18"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6043,11 +6212,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -6215,39 +6384,81 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="2"/>
+      <c r="A18" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B18" s="41">
+        <v>0.33</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B19" s="41">
+        <v>2.66</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="40">
+        <v>45278</v>
+      </c>
+      <c r="B20" s="41">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="2"/>
+      <c r="A21" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B21" s="41">
+        <v>2.5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="40">
+        <v>45299</v>
+      </c>
+      <c r="B22" s="41">
+        <v>1.5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>45306</v>
+      </c>
+      <c r="B23" s="41">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>45313</v>
+      </c>
+      <c r="B24" s="41">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>

</xml_diff>